<commit_message>
dokume phok my a$$
</commit_message>
<xml_diff>
--- a/Requis_Remise/Dictionnaires/Dictionnaire_Triggers.xlsx
+++ b/Requis_Remise/Dictionnaires/Dictionnaire_Triggers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t xml:space="preserve">TI_CAMISOLES                   </t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>Dictionnaire fait par Michaël Trahan</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>*ID - Insert transaction</t>
   </si>
 </sst>
 </file>
@@ -652,45 +658,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -707,11 +674,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -740,95 +835,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -843,13 +849,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A3:D36" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A3:D36" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A3:D36"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Nom" dataDxfId="4"/>
-    <tableColumn id="2" name="But" dataDxfId="3"/>
-    <tableColumn id="3" name="Spécification" dataDxfId="2"/>
-    <tableColumn id="4" name="Auteur" dataDxfId="1"/>
+    <tableColumn id="1" name="Nom" dataDxfId="3"/>
+    <tableColumn id="2" name="But" dataDxfId="2"/>
+    <tableColumn id="3" name="Spécification" dataDxfId="1"/>
+    <tableColumn id="4" name="Auteur" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1120,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,465 +1139,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="26" t="s">
-        <v>64</v>
+      <c r="D15" s="13" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="26" t="s">
-        <v>64</v>
+      <c r="D18" s="13" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32" t="s">
+      <c r="C36" s="18"/>
+      <c r="D36" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="20"/>
+      <c r="C39" s="32"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="21"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="21"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1606,50 +1612,50 @@
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="11"/>
+      <c r="C45" s="21"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="22"/>
+      <c r="C46" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>